<commit_message>
wangyifan 9/18 report 1
</commit_message>
<xml_diff>
--- a/ArticleReview/article_review (Diffusion).xlsx
+++ b/ArticleReview/article_review (Diffusion).xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeskTop\Accelerator-DiffusionModel\ArticleReview\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71DBE16-A8A8-4439-93F7-002ECDA41119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,14 +24,367 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Article</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contribution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DiffPattern: Layout Pattern Generation via Discrete Diffusion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Generate Different Patterns from Single Topology.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discrete Diffusion Model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DM-Tune: Quantizing Diffusion Models with
+Mixture-of-Gaussian Guided Noise Tuning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DINOv2-ViT (feature extractor)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solved Problem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Generated images</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>develop a novel layout pattern generation method based on
+discrete denoising for synthesizing layout topology</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hardware Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) a fine-grained mixed-precision
+strategy can surpass full-precision models (2)  integer-based strategies
+produce lower quality images. (3) 16-bit quantization offers a significant
+speedup with comparable performance to 32-bit and BF16
+generally outperforms FP16 (4) For low-precision, FP8 (E4M3) is preferred over
+FP8 (E5M2) for better performance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Efficient Continuous Logic Optimization with
+Diffusion Model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logic synthesis optimization</t>
+  </si>
+  <si>
+    <t>QoR surrogate model+diffusion model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>proposed method not
+only achieves lower area and delay but also improves efficiency
+by 5X to 130X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Late Breaking Results: A Diffusion-Based Framework for
+Configurable and Realistic Multi-Storage Trace Generation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EDA synthesis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>first work that utilizes the diffusion
+technique for the storage trace generation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diffusion-based synthetic trace generation
+framework</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Late Breaking Results: A Geometric Diffusion Model
+for Macro Placement Generation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Macro placement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MacroDiff,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduces
+macro overlap by 91.6%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Late Breaking Results: Customized Diffusion Model Empowered
+by Heterogeneous Graph Network for Effective Floorplanning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heterogeneous graph convolutional network
+(HGCN) and graph attention blocks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>customized diffusion model to
+directly generate high-quality initial floorplans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>floorplans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Late Breaking Results: Encoder-Decoder
+Generative Diffusion Transformer
+Towards Push-Button Analog IC Sizing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sizing
+of analog  circuits</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diffusion models (DMs) with an attention-based
+encoder-decoder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>presenting higher generalization capabilities
+to performance targets not seen during training</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MHDiff: Memory- and Hardware-Efficient Diffusion
+Acceleration via Focal Pixel Aware Quantization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) release memory burden (2)  high- and low-precision quantization for focal pixels others respectively (3) use a PE array to process the condensed high-precision
+data through minor modifications to the PE units.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pixel-adaptive quantization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HW-params</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>28nm, 500MHz, simwork</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Others</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compared with SOTA: Cambricon-D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MHDiff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RADiT: Redundancy-Aware Diffusion Transformer
+Acceleration Leveraging Timestep Similarity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redundancy-aware DiT
+(RADiT)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) identify data redundancy by evaluating
+blockwise input features and skip redundant computations by reusing results from consecutive timesteps (2) Dynamic Threshold Scaling Module
+(DTSM) and Compress and Compare Unit (CCU) are employed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DiT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compared with vanilla DiT hardware baseline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQ-DM: Accelerating Diffusion Models with
+Aggressive Quantization and Temporal Sparsity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Our 4-bit quantization technique demonstrates
+superior generation quality compared to existing 4-bit methods</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elucidated Diffusion
+Models, EDM [4] and EDM2 [5], as our baseline diffusion
+models</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CIFAR-10
+AFHQv2
+FFHQ
+ImageNet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>28nm, simwork</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In the future, we plan to extend our
+techniques to diffusion models targeting video generation [39]
+and apply our methodology to other generative models.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>We report on neural processing unit (NPU) in 4nm
+Samsung Exynos™ 2400 that employs heterogeneous architecture consisting of vector
+engines and two types of tensor engines</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>An On-Device Generative AI Focused Neural Processing Unit in
+4nm Flagship Mobile SoC with Fan-Out Wafer-Level Package</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chipwork</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Samsung Electronics, Hwaseong, Korea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A 28nm 74.34TFLOPS/W BF16 Heterogenous CIM-Based
+Accelerator Exploiting Denoising-Similarity for Diffusion
+Models</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISSCC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) CIM with 2-bit parallel (2) FP: OP_CIM; Man_Digital (3) in memory redundancy search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diffusion Model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>28nm, BF16/FP16, chipwork</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EdgeDiff: 418.4mJ/Inference Multi-Modal Few-Step Diffusion
+Model Accelerator with Mixed-Precision and Reordered Group
+Quantization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) increased precision demands with fewer denoising steps (2) mixed-precision and group quantization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text/image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>28nm, INT8/INT4/INT12, chipwork</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -37,7 +396,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,15 +404,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +716,382 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="15.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1"/>
+    <col min="4" max="4" width="39.125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="15.5" style="1"/>
+    <col min="7" max="7" width="74.75" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="15.5" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="114" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2024</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A12:A14"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>